<commit_message>
Lagde et filter for minimum inntekt for utbetalingstidslinjer
En person må ha inntekt over 0,5G/2G for å få sykepenger.

Co-authored-by: Stephen Ramthun <stephen.ramthun@nav.no>
Co-authored-by: Marthe Skogen <marthe.skogen@nav.no>
</commit_message>
<xml_diff>
--- a/doc/Spleis Unit Test Counts.xlsx
+++ b/doc/Spleis Unit Test Counts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/src/nav/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/src/nav/helse-spleis/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FA26E4-C53A-1A42-A91B-709B2F3CF724}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818FD83B-6CB6-8444-93E1-34AAF4DEC823}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27340" yWindow="5120" windowWidth="16320" windowHeight="14200" xr2:uid="{40FC2C12-094E-6140-8BF5-84A9E61F4CDF}"/>
   </bookViews>
@@ -213,26 +213,29 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>43728</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43791</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43803</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43810</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43817</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43832</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43839</c:v>
                 </c:pt>
               </c:numCache>
@@ -240,26 +243,29 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$7</c:f>
+              <c:f>Sheet1!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>28</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>22</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
@@ -308,26 +314,29 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>43728</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43791</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43803</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43810</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43817</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43832</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43839</c:v>
                 </c:pt>
               </c:numCache>
@@ -335,26 +344,29 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$7</c:f>
+              <c:f>Sheet1!$C$2:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>211</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>218</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>276</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>308</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>328</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>353</c:v>
                 </c:pt>
               </c:numCache>
@@ -1145,7 +1157,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1471,10 +1483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C39875-F38F-9346-8BC8-68FDF132B9B2}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1495,91 +1507,106 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>43791</v>
+        <v>43728</v>
       </c>
       <c r="B2">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>211</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <f>C2+B2</f>
-        <v>252</v>
+        <f t="shared" ref="D2:D3" si="0">C2+B2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>43803</v>
+        <v>43791</v>
       </c>
       <c r="B3">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C3">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="D3">
-        <f>C3+B3</f>
-        <v>258</v>
+        <f t="shared" si="0"/>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>43810</v>
+        <v>43803</v>
       </c>
       <c r="B4">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="C4">
-        <v>276</v>
+        <v>218</v>
       </c>
       <c r="D4">
-        <f>C4+B4</f>
-        <v>304</v>
+        <f t="shared" ref="D2:D8" si="1">C4+B4</f>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>43817</v>
+        <v>43810</v>
       </c>
       <c r="B5">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C5">
-        <v>308</v>
+        <v>276</v>
       </c>
       <c r="D5">
-        <f>C5+B5</f>
-        <v>329</v>
+        <f t="shared" si="1"/>
+        <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>43832</v>
+        <v>43817</v>
       </c>
       <c r="B6">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6">
-        <v>328</v>
+        <v>308</v>
       </c>
       <c r="D6">
-        <f>C6+B6</f>
-        <v>350</v>
+        <f t="shared" si="1"/>
+        <v>329</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
+        <v>43832</v>
+      </c>
+      <c r="B7">
+        <v>22</v>
+      </c>
+      <c r="C7">
+        <v>328</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>350</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>43839</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>25</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>353</v>
       </c>
-      <c r="D7">
-        <f>C7+B7</f>
+      <c r="D8">
+        <f t="shared" si="1"/>
         <v>378</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Created new assertions in NySøknadHendelseTest using a PersonVisitor as an alternative to a PersonObserver.
</commit_message>
<xml_diff>
--- a/doc/Spleis Unit Test Counts.xlsx
+++ b/doc/Spleis Unit Test Counts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/src/nav/helse-spleis/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818FD83B-6CB6-8444-93E1-34AAF4DEC823}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D04E334-E303-BF48-B5AE-EDEA05EC18E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27340" yWindow="5120" windowWidth="16320" windowHeight="14200" xr2:uid="{40FC2C12-094E-6140-8BF5-84A9E61F4CDF}"/>
   </bookViews>
@@ -174,7 +174,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nb-NO"/>
+          <a:endParaRPr lang="en-NO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -424,7 +424,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nb-NO"/>
+            <a:endParaRPr lang="en-NO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="795730911"/>
@@ -482,7 +482,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nb-NO"/>
+            <a:endParaRPr lang="en-NO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="759151391"/>
@@ -524,7 +524,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nb-NO"/>
+          <a:endParaRPr lang="en-NO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -561,7 +561,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nb-NO"/>
+      <a:endParaRPr lang="en-NO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1483,10 +1483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C39875-F38F-9346-8BC8-68FDF132B9B2}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1546,7 +1546,7 @@
         <v>218</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D2:D8" si="1">C4+B4</f>
+        <f t="shared" ref="D4:D8" si="1">C4+B4</f>
         <v>258</v>
       </c>
     </row>
@@ -1608,6 +1608,11 @@
       <c r="D8">
         <f t="shared" si="1"/>
         <v>378</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>43846</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added timestamps for entries in Problemer.
</commit_message>
<xml_diff>
--- a/doc/Spleis Unit Test Counts.xlsx
+++ b/doc/Spleis Unit Test Counts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/src/nav/helse-spleis/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D04E334-E303-BF48-B5AE-EDEA05EC18E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A25C8B2-5163-9F47-8035-D2B59EBB0938}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27340" yWindow="5120" windowWidth="16320" windowHeight="14200" xr2:uid="{40FC2C12-094E-6140-8BF5-84A9E61F4CDF}"/>
   </bookViews>
@@ -213,10 +213,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>43728</c:v>
                 </c:pt>
@@ -237,16 +237,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>43839</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43846</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:f>Sheet1!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -267,6 +270,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -314,10 +320,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>43728</c:v>
                 </c:pt>
@@ -338,16 +344,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>43839</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43846</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$8</c:f>
+              <c:f>Sheet1!$C$2:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -368,6 +377,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>353</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>391</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1157,7 +1169,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1483,10 +1495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C39875-F38F-9346-8BC8-68FDF132B9B2}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1546,7 +1558,7 @@
         <v>218</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D8" si="1">C4+B4</f>
+        <f t="shared" ref="D4:D9" si="1">C4+B4</f>
         <v>258</v>
       </c>
     </row>
@@ -1606,7 +1618,7 @@
         <v>353</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D8" si="2">C8+B8</f>
         <v>378</v>
       </c>
     </row>
@@ -1614,6 +1626,19 @@
       <c r="A9" s="1">
         <v>43846</v>
       </c>
+      <c r="B9">
+        <v>44</v>
+      </c>
+      <c r="C9">
+        <v>391</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>435</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Renamed "help" in Aktivitetslogger to "need" to better reflect the assistance required from caseworkers
Co-authored-by: Richard Martinsen <richard.martinsen@nav.no>
</commit_message>
<xml_diff>
--- a/doc/Spleis Unit Test Counts.xlsx
+++ b/doc/Spleis Unit Test Counts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/src/nav/helse-spleis/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A25C8B2-5163-9F47-8035-D2B59EBB0938}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB4D2E4-DA94-E840-BA48-41A451036CA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27340" yWindow="5120" windowWidth="16320" windowHeight="14200" xr2:uid="{40FC2C12-094E-6140-8BF5-84A9E61F4CDF}"/>
   </bookViews>
@@ -1495,10 +1495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C39875-F38F-9346-8BC8-68FDF132B9B2}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1558,7 +1558,7 @@
         <v>218</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D9" si="1">C4+B4</f>
+        <f t="shared" ref="D4:D10" si="1">C4+B4</f>
         <v>258</v>
       </c>
     </row>
@@ -1638,7 +1638,34 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1">
+        <v>43853</v>
+      </c>
+      <c r="B10">
+        <v>46</v>
+      </c>
+      <c r="C10">
+        <v>418</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>464</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>43860</v>
+      </c>
+      <c r="B11">
+        <v>47</v>
+      </c>
+      <c r="C11">
+        <v>426</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ref="D11" si="3">C11+B11</f>
+        <v>473</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Unit Test Counts
</commit_message>
<xml_diff>
--- a/doc/Spleis Unit Test Counts.xlsx
+++ b/doc/Spleis Unit Test Counts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/src/nav/helse-spleis/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB4D2E4-DA94-E840-BA48-41A451036CA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6818807C-888D-DB42-BC73-1D5682188CF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27340" yWindow="5120" windowWidth="16320" windowHeight="14200" xr2:uid="{40FC2C12-094E-6140-8BF5-84A9E61F4CDF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Model</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -1495,10 +1498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C39875-F38F-9346-8BC8-68FDF132B9B2}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1667,6 +1670,11 @@
         <v>473</v>
       </c>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Removed old Aktivitetslogger and supporting classes and tests.
</commit_message>
<xml_diff>
--- a/doc/Spleis Unit Test Counts.xlsx
+++ b/doc/Spleis Unit Test Counts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/src/nav/helse-spleis/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6818807C-888D-DB42-BC73-1D5682188CF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD44BB32-BF49-3146-BD2A-79DD9CE0E9FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27340" yWindow="5120" windowWidth="16320" windowHeight="14200" xr2:uid="{40FC2C12-094E-6140-8BF5-84A9E61F4CDF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Model</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Rapids</t>
   </si>
 </sst>
 </file>
@@ -188,10 +191,122 @@
         <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="2"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Unit Test Counts</c:v>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rapids</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="ltUpDiag">
+              <a:fgClr>
+                <a:schemeClr val="accent3"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent3"/>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>43728</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43791</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43803</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43810</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43817</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43832</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43839</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43846</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43853</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43860</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43867</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43874</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43881</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43888</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="13">
+                  <c:v>35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B4AD-1D48-B8E3-FA6E6F6B9056}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mediator</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:pattFill prst="ltUpDiag">
@@ -216,10 +331,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:f>Sheet1!$A$2:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>43728</c:v>
                 </c:pt>
@@ -243,16 +358,34 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>43846</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43853</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43860</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43867</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43874</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43881</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43888</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$9</c:f>
+              <c:f>Sheet1!$C$2:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -276,6 +409,24 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -288,10 +439,10 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Sheet1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -323,10 +474,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:f>Sheet1!$A$2:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>43728</c:v>
                 </c:pt>
@@ -350,16 +501,34 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>43846</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43853</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43860</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43867</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43874</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43881</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43888</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$9</c:f>
+              <c:f>Sheet1!$D$2:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -383,6 +552,24 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>391</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>418</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>426</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>347</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>362</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>372</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>380</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1164,15 +1351,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>196850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1498,180 +1685,246 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C39875-F38F-9346-8BC8-68FDF132B9B2}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43728</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D3" si="0">C2+B2</f>
         <v>0</v>
       </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E3" si="0">D2+C2</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43791</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>41</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>211</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <f t="shared" si="0"/>
         <v>252</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43803</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>40</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>218</v>
       </c>
-      <c r="D4">
-        <f t="shared" ref="D4:D10" si="1">C4+B4</f>
+      <c r="E4">
+        <f t="shared" ref="E4:E13" si="1">D4+C4</f>
         <v>258</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43810</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>28</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>276</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <f t="shared" si="1"/>
         <v>304</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43817</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>21</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>308</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <f t="shared" si="1"/>
         <v>329</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43832</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>22</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>328</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <f t="shared" si="1"/>
         <v>350</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43839</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>25</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>353</v>
       </c>
-      <c r="D8">
-        <f t="shared" ref="D8" si="2">C8+B8</f>
+      <c r="E8">
+        <f t="shared" ref="E8" si="2">D8+C8</f>
         <v>378</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43846</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>44</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>391</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <f t="shared" si="1"/>
         <v>435</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43853</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>46</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>418</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <f t="shared" si="1"/>
         <v>464</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43860</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>47</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>426</v>
       </c>
-      <c r="D11">
-        <f t="shared" ref="D11" si="3">C11+B11</f>
+      <c r="E11">
+        <f t="shared" ref="E11" si="3">D11+C11</f>
         <v>473</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C15" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>43867</v>
+      </c>
+      <c r="C12">
+        <v>48</v>
+      </c>
+      <c r="D12">
+        <v>347</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>395</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>43874</v>
+      </c>
+      <c r="C13">
+        <v>48</v>
+      </c>
+      <c r="D13">
+        <v>362</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>410</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>43881</v>
+      </c>
+      <c r="C14">
+        <v>45</v>
+      </c>
+      <c r="D14">
+        <v>372</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ref="E14" si="4">D14+C14</f>
+        <v>417</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>43888</v>
+      </c>
+      <c r="B15">
+        <v>35</v>
+      </c>
+      <c r="C15">
+        <v>33</v>
+      </c>
+      <c r="D15">
+        <v>380</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ref="E15" si="5">D15+C15</f>
+        <v>413</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>